<commit_message>
image for doc uploads
</commit_message>
<xml_diff>
--- a/examples/chp/chp_data.xlsx
+++ b/examples/chp/chp_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Time-Series" sheetId="2" r:id="rId1"/>
@@ -404,7 +404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1356,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>